<commit_message>
chore: update svt list
</commit_message>
<xml_diff>
--- a/webcrawler/data/4_servents.xlsx
+++ b/webcrawler/data/4_servents.xlsx
@@ -5135,7 +5135,11 @@
           <t>耀星哈桑</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr"/>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>耀星的哈桑</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -5159,7 +5163,11 @@
           <t>亞歷山德羅·迪·卡利奧斯特羅</t>
         </is>
       </c>
-      <c r="F169" t="inlineStr"/>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>亞歷山德羅．迪．卡廖斯特羅</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -5370,7 +5378,11 @@
           <t>アビゲイル・ウィリアムズ〔サンタ〕</t>
         </is>
       </c>
-      <c r="E178" t="inlineStr"/>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>阿比蓋爾·威廉姆斯〔聖誕〕</t>
+        </is>
+      </c>
       <c r="F178" t="inlineStr"/>
     </row>
     <row r="179">

</xml_diff>